<commit_message>
Simulated binary CX works
</commit_message>
<xml_diff>
--- a/deap/tests/nsga1_zdt1_Xbinary_Mbinary.xlsx
+++ b/deap/tests/nsga1_zdt1_Xbinary_Mbinary.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="17490" windowHeight="6900" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="17490" windowHeight="6900" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="3" r:id="rId1"/>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="77">
   <si>
     <t>Yes</t>
   </si>
@@ -113,9 +113,6 @@
   </si>
   <si>
     <t>float</t>
-  </si>
-  <si>
-    <t>var0</t>
   </si>
   <si>
     <t>var1</t>
@@ -690,23 +687,23 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B3" t="str">
         <f>CONCATENATE(B1,"\",B2)</f>
@@ -715,7 +712,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B4" t="s">
         <v>0</v>
@@ -723,7 +720,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B5" t="s">
         <v>1</v>
@@ -731,7 +728,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B6" t="s">
         <v>1</v>
@@ -748,24 +745,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C1" t="s">
         <v>65</v>
-      </c>
-      <c r="C1" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -776,7 +773,7 @@
         <v>40</v>
       </c>
       <c r="C2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -787,12 +784,12 @@
         <v>250</v>
       </c>
       <c r="C3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B4">
         <v>0.5</v>
@@ -803,7 +800,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B5">
         <v>0.5</v>
@@ -814,18 +811,18 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B6">
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B7">
         <v>0.5</v>
@@ -836,7 +833,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B8">
         <v>0.05</v>
@@ -866,35 +863,35 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" t="s">
         <v>54</v>
-      </c>
-      <c r="B1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C1" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C3" t="s">
         <v>60</v>
-      </c>
-      <c r="C3" t="s">
-        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -907,8 +904,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -920,35 +917,35 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B3" t="s">
         <v>67</v>
       </c>
-      <c r="B3" t="s">
-        <v>68</v>
-      </c>
       <c r="C3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -958,10 +955,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView zoomScale="130" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1496,23 +1493,6 @@
         <v>0.01</v>
       </c>
       <c r="E31" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>45</v>
-      </c>
-      <c r="B32" t="s">
-        <v>14</v>
-      </c>
-      <c r="C32" s="3">
-        <v>0</v>
-      </c>
-      <c r="D32" s="3">
-        <v>0.01</v>
-      </c>
-      <c r="E32" s="3">
         <v>1</v>
       </c>
     </row>
@@ -1594,7 +1574,7 @@
         <v>9</v>
       </c>
       <c r="B1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Mutation fixed Found problem with convergence - See Revisisting Diversity papers by DEAP authors
</commit_message>
<xml_diff>
--- a/deap/tests/nsga1_zdt1_Xbinary_Mbinary.xlsx
+++ b/deap/tests/nsga1_zdt1_Xbinary_Mbinary.xlsx
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="76">
   <si>
     <t>Yes</t>
   </si>
@@ -241,9 +241,6 @@
     <t>select</t>
   </si>
   <si>
-    <t>mj_random_jump</t>
-  </si>
-  <si>
     <t>mj_zdt1_decimal</t>
   </si>
   <si>
@@ -283,12 +280,6 @@
     <t>mate</t>
   </si>
   <si>
-    <t>Probability flip allele</t>
-  </si>
-  <si>
-    <t>Jump size</t>
-  </si>
-  <si>
     <t>Probability mutation</t>
   </si>
   <si>
@@ -299,6 +290,12 @@
   </si>
   <si>
     <t>mj_cxSimulatedBinaryBounded</t>
+  </si>
+  <si>
+    <t>mj_mutPolynomialBounded</t>
+  </si>
+  <si>
+    <t>indpb</t>
   </si>
 </sst>
 </file>
@@ -355,7 +352,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -372,6 +369,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -728,7 +726,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B6" t="s">
         <v>1</v>
@@ -743,10 +741,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -759,10 +757,10 @@
         <v>53</v>
       </c>
       <c r="B1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" t="s">
         <v>64</v>
-      </c>
-      <c r="C1" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -773,7 +771,7 @@
         <v>40</v>
       </c>
       <c r="C2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -784,15 +782,15 @@
         <v>250</v>
       </c>
       <c r="C3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B4">
-        <v>0.5</v>
+        <v>0.9</v>
       </c>
       <c r="C4" t="s">
         <v>14</v>
@@ -800,10 +798,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B5">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="C5" t="s">
         <v>14</v>
@@ -814,31 +812,20 @@
         <v>72</v>
       </c>
       <c r="B6">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C6" t="s">
-        <v>63</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>73</v>
-      </c>
-      <c r="B7">
-        <v>0.5</v>
+        <v>75</v>
+      </c>
+      <c r="B7" s="8">
+        <v>3.3333333333333333E-2</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>75</v>
-      </c>
-      <c r="B8">
-        <v>0.05</v>
-      </c>
-      <c r="C8" t="s">
         <v>14</v>
       </c>
     </row>
@@ -866,7 +853,7 @@
         <v>53</v>
       </c>
       <c r="B1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C1" t="s">
         <v>54</v>
@@ -877,10 +864,10 @@
         <v>55</v>
       </c>
       <c r="B2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -888,10 +875,10 @@
         <v>56</v>
       </c>
       <c r="B3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C3" t="s">
         <v>59</v>
-      </c>
-      <c r="C3" t="s">
-        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -920,32 +907,32 @@
         <v>56</v>
       </c>
       <c r="B1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B3" t="s">
         <v>66</v>
       </c>
-      <c r="B3" t="s">
-        <v>67</v>
-      </c>
       <c r="C3" t="s">
-        <v>57</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>